<commit_message>
Formatted legis2017 results & saved concatenated file
</commit_message>
<xml_diff>
--- a/fondamentaux/data/results_by_arrdmt.xlsx
+++ b/fondamentaux/data/results_by_arrdmt.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:M81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,6 +426,11 @@
           <t>other</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -466,6 +471,11 @@
       <c r="L2" t="n">
         <v>0</v>
       </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -504,13 +514,18 @@
       <c r="L3" t="n">
         <v>153</v>
       </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>39591</v>
+        <v>42848</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -518,31 +533,34 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>6736</v>
+        <v>9026</v>
       </c>
       <c r="F4" t="n">
-        <v>90</v>
+        <v>1231</v>
       </c>
       <c r="G4" t="n">
-        <v>2231</v>
-      </c>
-      <c r="H4" t="n">
-        <v>2016</v>
-      </c>
+        <v>659</v>
+      </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="n">
-        <v>621</v>
+        <v>3561</v>
       </c>
       <c r="J4" t="n">
-        <v>1543</v>
+        <v>2831</v>
       </c>
       <c r="K4" t="n">
-        <v>167</v>
+        <v>443</v>
       </c>
       <c r="L4" t="n">
-        <v>68</v>
+        <v>301</v>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>president</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -550,7 +568,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>41723</v>
+        <v>42897</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -558,29 +576,36 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>6857</v>
+        <v>6282</v>
       </c>
       <c r="F5" t="n">
-        <v>192</v>
+        <v>434</v>
       </c>
       <c r="G5" t="n">
-        <v>1565</v>
+        <v>418</v>
       </c>
       <c r="H5" t="n">
-        <v>2260</v>
-      </c>
-      <c r="I5" t="inlineStr"/>
+        <v>363</v>
+      </c>
+      <c r="I5" t="n">
+        <v>2958</v>
+      </c>
       <c r="J5" t="n">
-        <v>1663</v>
+        <v>1525</v>
       </c>
       <c r="K5" t="n">
-        <v>272</v>
+        <v>148</v>
       </c>
       <c r="L5" t="n">
-        <v>905</v>
+        <v>436</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>legislative</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -596,31 +621,36 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6" t="n">
-        <v>11974</v>
+        <v>6736</v>
       </c>
       <c r="F6" t="n">
-        <v>225</v>
+        <v>90</v>
       </c>
       <c r="G6" t="n">
-        <v>6685</v>
+        <v>2231</v>
       </c>
       <c r="H6" t="n">
-        <v>1237</v>
+        <v>2016</v>
       </c>
       <c r="I6" t="n">
-        <v>1111</v>
+        <v>621</v>
       </c>
       <c r="J6" t="n">
-        <v>2458</v>
+        <v>1543</v>
       </c>
       <c r="K6" t="n">
-        <v>258</v>
+        <v>167</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>68</v>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -636,29 +666,34 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7" t="n">
-        <v>11615</v>
+        <v>6857</v>
       </c>
       <c r="F7" t="n">
-        <v>464</v>
+        <v>192</v>
       </c>
       <c r="G7" t="n">
-        <v>5493</v>
+        <v>1565</v>
       </c>
       <c r="H7" t="n">
-        <v>1252</v>
+        <v>2260</v>
       </c>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="n">
-        <v>3379</v>
+        <v>1663</v>
       </c>
       <c r="K7" t="n">
-        <v>580</v>
+        <v>272</v>
       </c>
       <c r="L7" t="n">
-        <v>447</v>
+        <v>905</v>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -666,7 +701,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>39591</v>
+        <v>42848</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -674,31 +709,34 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E8" t="n">
-        <v>10573</v>
+        <v>11292</v>
       </c>
       <c r="F8" t="n">
-        <v>151</v>
+        <v>1802</v>
       </c>
       <c r="G8" t="n">
-        <v>5127</v>
-      </c>
-      <c r="H8" t="n">
-        <v>834</v>
-      </c>
+        <v>1099</v>
+      </c>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="n">
-        <v>863</v>
+        <v>5014</v>
       </c>
       <c r="J8" t="n">
-        <v>3312</v>
+        <v>2640</v>
       </c>
       <c r="K8" t="n">
-        <v>286</v>
+        <v>399</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>338</v>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>president</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -706,7 +744,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>41723</v>
+        <v>42897</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -714,29 +752,36 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E9" t="n">
-        <v>9850</v>
+        <v>7560</v>
       </c>
       <c r="F9" t="n">
-        <v>376</v>
+        <v>601</v>
       </c>
       <c r="G9" t="n">
-        <v>3684</v>
+        <v>563</v>
       </c>
       <c r="H9" t="n">
-        <v>916</v>
-      </c>
-      <c r="I9" t="inlineStr"/>
+        <v>810</v>
+      </c>
+      <c r="I9" t="n">
+        <v>4004</v>
+      </c>
       <c r="J9" t="n">
-        <v>3725</v>
+        <v>843</v>
       </c>
       <c r="K9" t="n">
-        <v>512</v>
+        <v>147</v>
       </c>
       <c r="L9" t="n">
-        <v>637</v>
+        <v>592</v>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>legislative</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -752,31 +797,36 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E10" t="n">
-        <v>23614</v>
+        <v>11974</v>
       </c>
       <c r="F10" t="n">
-        <v>688</v>
+        <v>225</v>
       </c>
       <c r="G10" t="n">
-        <v>8187</v>
+        <v>6685</v>
       </c>
       <c r="H10" t="n">
-        <v>1287</v>
+        <v>1237</v>
       </c>
       <c r="I10" t="n">
-        <v>3385</v>
+        <v>1111</v>
       </c>
       <c r="J10" t="n">
-        <v>8958</v>
+        <v>2458</v>
       </c>
       <c r="K10" t="n">
-        <v>418</v>
+        <v>258</v>
       </c>
       <c r="L10" t="n">
-        <v>691</v>
+        <v>0</v>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -792,29 +842,34 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E11" t="n">
-        <v>22243</v>
+        <v>11615</v>
       </c>
       <c r="F11" t="n">
-        <v>976</v>
+        <v>464</v>
       </c>
       <c r="G11" t="n">
-        <v>7550</v>
+        <v>5493</v>
       </c>
       <c r="H11" t="n">
-        <v>1985</v>
+        <v>1252</v>
       </c>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="n">
-        <v>6336</v>
+        <v>3379</v>
       </c>
       <c r="K11" t="n">
-        <v>805</v>
+        <v>580</v>
       </c>
       <c r="L11" t="n">
-        <v>4591</v>
+        <v>447</v>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -822,7 +877,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>39591</v>
+        <v>42848</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -830,29 +885,34 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E12" t="n">
-        <v>15488</v>
-      </c>
-      <c r="F12" t="inlineStr"/>
+        <v>18485</v>
+      </c>
+      <c r="F12" t="n">
+        <v>3078</v>
+      </c>
       <c r="G12" t="n">
-        <v>5166</v>
-      </c>
-      <c r="H12" t="n">
-        <v>590</v>
-      </c>
+        <v>1963</v>
+      </c>
+      <c r="H12" t="inlineStr"/>
       <c r="I12" t="n">
-        <v>1530</v>
+        <v>8325</v>
       </c>
       <c r="J12" t="n">
-        <v>7269</v>
+        <v>3994</v>
       </c>
       <c r="K12" t="n">
-        <v>356</v>
+        <v>615</v>
       </c>
       <c r="L12" t="n">
-        <v>577</v>
+        <v>510</v>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>president</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -860,7 +920,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>41723</v>
+        <v>42897</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -868,29 +928,36 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E13" t="n">
-        <v>14759</v>
+        <v>13014</v>
       </c>
       <c r="F13" t="n">
-        <v>349</v>
+        <v>1035</v>
       </c>
       <c r="G13" t="n">
-        <v>3855</v>
+        <v>1637</v>
       </c>
       <c r="H13" t="n">
-        <v>982</v>
-      </c>
-      <c r="I13" t="inlineStr"/>
+        <v>1299</v>
+      </c>
+      <c r="I13" t="n">
+        <v>6513</v>
+      </c>
       <c r="J13" t="n">
-        <v>7766</v>
+        <v>1231</v>
       </c>
       <c r="K13" t="n">
-        <v>708</v>
+        <v>340</v>
       </c>
       <c r="L13" t="n">
-        <v>1099</v>
+        <v>959</v>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>legislative</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -906,29 +973,36 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E14" t="n">
-        <v>17967</v>
-      </c>
-      <c r="F14" t="inlineStr"/>
+        <v>10573</v>
+      </c>
+      <c r="F14" t="n">
+        <v>151</v>
+      </c>
       <c r="G14" t="n">
-        <v>4080</v>
+        <v>5127</v>
       </c>
       <c r="H14" t="n">
-        <v>535</v>
+        <v>834</v>
       </c>
       <c r="I14" t="n">
-        <v>2819</v>
+        <v>863</v>
       </c>
       <c r="J14" t="n">
-        <v>8894</v>
+        <v>3312</v>
       </c>
       <c r="K14" t="n">
-        <v>537</v>
+        <v>286</v>
       </c>
       <c r="L14" t="n">
-        <v>1102</v>
+        <v>0</v>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -944,29 +1018,34 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E15" t="n">
-        <v>17910</v>
+        <v>9850</v>
       </c>
       <c r="F15" t="n">
-        <v>198</v>
+        <v>376</v>
       </c>
       <c r="G15" t="n">
-        <v>3031</v>
+        <v>3684</v>
       </c>
       <c r="H15" t="n">
-        <v>546</v>
+        <v>916</v>
       </c>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="n">
-        <v>7345</v>
+        <v>3725</v>
       </c>
       <c r="K15" t="n">
-        <v>1066</v>
+        <v>512</v>
       </c>
       <c r="L15" t="n">
-        <v>5724</v>
+        <v>637</v>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -974,7 +1053,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>39591</v>
+        <v>42848</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -982,29 +1061,34 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E16" t="n">
-        <v>12325</v>
-      </c>
-      <c r="F16" t="inlineStr"/>
+        <v>15106</v>
+      </c>
+      <c r="F16" t="n">
+        <v>2329</v>
+      </c>
       <c r="G16" t="n">
-        <v>2302</v>
-      </c>
-      <c r="H16" t="n">
-        <v>318</v>
-      </c>
+        <v>1370</v>
+      </c>
+      <c r="H16" t="inlineStr"/>
       <c r="I16" t="n">
-        <v>808</v>
+        <v>6182</v>
       </c>
       <c r="J16" t="n">
-        <v>4119</v>
+        <v>3956</v>
       </c>
       <c r="K16" t="n">
-        <v>293</v>
+        <v>735</v>
       </c>
       <c r="L16" t="n">
-        <v>4485</v>
+        <v>534</v>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>president</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -1012,7 +1096,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>41723</v>
+        <v>42897</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -1020,29 +1104,36 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E17" t="n">
-        <v>12622</v>
+        <v>10549</v>
       </c>
       <c r="F17" t="n">
-        <v>178</v>
+        <v>882</v>
       </c>
       <c r="G17" t="n">
-        <v>1944</v>
+        <v>1176</v>
       </c>
       <c r="H17" t="n">
-        <v>442</v>
-      </c>
-      <c r="I17" t="inlineStr"/>
+        <v>563</v>
+      </c>
+      <c r="I17" t="n">
+        <v>4612</v>
+      </c>
       <c r="J17" t="n">
-        <v>5884</v>
+        <v>1779</v>
       </c>
       <c r="K17" t="n">
-        <v>602</v>
+        <v>289</v>
       </c>
       <c r="L17" t="n">
-        <v>3572</v>
+        <v>1248</v>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>legislative</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -1058,31 +1149,36 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E18" t="n">
-        <v>20643</v>
+        <v>23614</v>
       </c>
       <c r="F18" t="n">
-        <v>602</v>
+        <v>688</v>
       </c>
       <c r="G18" t="n">
-        <v>10163</v>
+        <v>8187</v>
       </c>
       <c r="H18" t="n">
-        <v>1299</v>
+        <v>1287</v>
       </c>
       <c r="I18" t="n">
-        <v>1659</v>
+        <v>3385</v>
       </c>
       <c r="J18" t="n">
-        <v>6353</v>
+        <v>8958</v>
       </c>
       <c r="K18" t="n">
-        <v>567</v>
+        <v>418</v>
       </c>
       <c r="L18" t="n">
-        <v>0</v>
+        <v>691</v>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -1098,29 +1194,34 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E19" t="n">
-        <v>20751</v>
+        <v>22243</v>
       </c>
       <c r="F19" t="n">
-        <v>772</v>
+        <v>976</v>
       </c>
       <c r="G19" t="n">
-        <v>8125</v>
+        <v>7550</v>
       </c>
       <c r="H19" t="n">
-        <v>1663</v>
+        <v>1985</v>
       </c>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="n">
-        <v>8181</v>
+        <v>6336</v>
       </c>
       <c r="K19" t="n">
-        <v>1010</v>
+        <v>805</v>
       </c>
       <c r="L19" t="n">
-        <v>1000</v>
+        <v>4591</v>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -1128,7 +1229,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>39591</v>
+        <v>42848</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -1136,31 +1237,34 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E20" t="n">
-        <v>28359</v>
+        <v>31008</v>
       </c>
       <c r="F20" t="n">
-        <v>2158</v>
+        <v>4960</v>
       </c>
       <c r="G20" t="n">
-        <v>13766</v>
-      </c>
-      <c r="H20" t="n">
-        <v>2564</v>
-      </c>
+        <v>3103</v>
+      </c>
+      <c r="H20" t="inlineStr"/>
       <c r="I20" t="n">
-        <v>2348</v>
+        <v>12316</v>
       </c>
       <c r="J20" t="n">
-        <v>4513</v>
+        <v>8273</v>
       </c>
       <c r="K20" t="n">
-        <v>837</v>
+        <v>1225</v>
       </c>
       <c r="L20" t="n">
-        <v>2173</v>
+        <v>1131</v>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>president</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -1168,7 +1272,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>41723</v>
+        <v>42897</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -1176,29 +1280,36 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E21" t="n">
-        <v>26993</v>
+        <v>22755</v>
       </c>
       <c r="F21" t="n">
-        <v>1730</v>
+        <v>1947</v>
       </c>
       <c r="G21" t="n">
-        <v>11973</v>
+        <v>1980</v>
       </c>
       <c r="H21" t="n">
-        <v>3102</v>
-      </c>
-      <c r="I21" t="inlineStr"/>
+        <v>1562</v>
+      </c>
+      <c r="I21" t="n">
+        <v>9379</v>
+      </c>
       <c r="J21" t="n">
-        <v>5798</v>
+        <v>3523</v>
       </c>
       <c r="K21" t="n">
-        <v>1460</v>
+        <v>543</v>
       </c>
       <c r="L21" t="n">
-        <v>2930</v>
+        <v>3821</v>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>legislative</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -1214,31 +1325,34 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E22" t="n">
-        <v>47031</v>
-      </c>
-      <c r="F22" t="n">
-        <v>2672</v>
-      </c>
+        <v>15488</v>
+      </c>
+      <c r="F22" t="inlineStr"/>
       <c r="G22" t="n">
-        <v>25894</v>
+        <v>5166</v>
       </c>
       <c r="H22" t="n">
-        <v>3726</v>
+        <v>590</v>
       </c>
       <c r="I22" t="n">
-        <v>4067</v>
+        <v>1530</v>
       </c>
       <c r="J22" t="n">
-        <v>9315</v>
+        <v>7269</v>
       </c>
       <c r="K22" t="n">
-        <v>1357</v>
+        <v>356</v>
       </c>
       <c r="L22" t="n">
-        <v>0</v>
+        <v>577</v>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -1254,29 +1368,34 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E23" t="n">
-        <v>45861</v>
+        <v>14759</v>
       </c>
       <c r="F23" t="n">
-        <v>2879</v>
+        <v>349</v>
       </c>
       <c r="G23" t="n">
-        <v>20524</v>
+        <v>3855</v>
       </c>
       <c r="H23" t="n">
-        <v>5301</v>
+        <v>982</v>
       </c>
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="n">
-        <v>12304</v>
+        <v>7766</v>
       </c>
       <c r="K23" t="n">
-        <v>2512</v>
+        <v>708</v>
       </c>
       <c r="L23" t="n">
-        <v>2341</v>
+        <v>1099</v>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -1284,7 +1403,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>39591</v>
+        <v>42848</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1292,31 +1411,34 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E24" t="n">
-        <v>53146</v>
+        <v>22332</v>
       </c>
       <c r="F24" t="n">
-        <v>2324</v>
+        <v>2038</v>
       </c>
       <c r="G24" t="n">
-        <v>24486</v>
-      </c>
-      <c r="H24" t="n">
-        <v>3125</v>
-      </c>
+        <v>1419</v>
+      </c>
+      <c r="H24" t="inlineStr"/>
       <c r="I24" t="n">
-        <v>5287</v>
+        <v>8729</v>
       </c>
       <c r="J24" t="n">
-        <v>12922</v>
+        <v>8769</v>
       </c>
       <c r="K24" t="n">
-        <v>1550</v>
+        <v>719</v>
       </c>
       <c r="L24" t="n">
-        <v>3452</v>
+        <v>658</v>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>president</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -1324,7 +1446,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>41723</v>
+        <v>42897</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1332,29 +1454,36 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E25" t="n">
-        <v>49695</v>
+        <v>15915</v>
       </c>
       <c r="F25" t="n">
-        <v>2678</v>
+        <v>688</v>
       </c>
       <c r="G25" t="n">
-        <v>18585</v>
+        <v>997</v>
       </c>
       <c r="H25" t="n">
-        <v>5001</v>
-      </c>
-      <c r="I25" t="inlineStr"/>
+        <v>764</v>
+      </c>
+      <c r="I25" t="n">
+        <v>7025</v>
+      </c>
       <c r="J25" t="n">
-        <v>16569</v>
+        <v>3455</v>
       </c>
       <c r="K25" t="n">
-        <v>3362</v>
+        <v>306</v>
       </c>
       <c r="L25" t="n">
-        <v>3500</v>
+        <v>2680</v>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>legislative</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -1370,31 +1499,34 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E26" t="n">
-        <v>58837</v>
-      </c>
-      <c r="F26" t="n">
-        <v>4608</v>
-      </c>
+        <v>17967</v>
+      </c>
+      <c r="F26" t="inlineStr"/>
       <c r="G26" t="n">
-        <v>29324</v>
+        <v>4080</v>
       </c>
       <c r="H26" t="n">
-        <v>3808</v>
+        <v>535</v>
       </c>
       <c r="I26" t="n">
-        <v>5320</v>
+        <v>2819</v>
       </c>
       <c r="J26" t="n">
-        <v>12559</v>
+        <v>8894</v>
       </c>
       <c r="K26" t="n">
-        <v>1989</v>
+        <v>537</v>
       </c>
       <c r="L26" t="n">
-        <v>1229</v>
+        <v>1102</v>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
       </c>
     </row>
     <row r="27">
@@ -1410,29 +1542,34 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>56670</v>
+        <v>17910</v>
       </c>
       <c r="F27" t="n">
-        <v>3326</v>
+        <v>198</v>
       </c>
       <c r="G27" t="n">
-        <v>25193</v>
+        <v>3031</v>
       </c>
       <c r="H27" t="n">
-        <v>5567</v>
+        <v>546</v>
       </c>
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="n">
-        <v>14157</v>
+        <v>7345</v>
       </c>
       <c r="K27" t="n">
-        <v>4229</v>
+        <v>1066</v>
       </c>
       <c r="L27" t="n">
-        <v>4198</v>
+        <v>5724</v>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
       </c>
     </row>
     <row r="28">
@@ -1440,7 +1577,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>39591</v>
+        <v>42848</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1448,31 +1585,34 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E28" t="n">
-        <v>48193</v>
+        <v>27798</v>
       </c>
       <c r="F28" t="n">
-        <v>1806</v>
+        <v>1552</v>
       </c>
       <c r="G28" t="n">
-        <v>21699</v>
-      </c>
-      <c r="H28" t="n">
-        <v>3871</v>
-      </c>
+        <v>1068</v>
+      </c>
+      <c r="H28" t="inlineStr"/>
       <c r="I28" t="n">
-        <v>6711</v>
+        <v>8785</v>
       </c>
       <c r="J28" t="n">
-        <v>11465</v>
+        <v>14650</v>
       </c>
       <c r="K28" t="n">
-        <v>1457</v>
+        <v>1064</v>
       </c>
       <c r="L28" t="n">
-        <v>1184</v>
+        <v>679</v>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>president</t>
+        </is>
       </c>
     </row>
     <row r="29">
@@ -1480,7 +1620,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="2" t="n">
-        <v>41723</v>
+        <v>42897</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1488,29 +1628,36 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E29" t="n">
-        <v>47477</v>
+        <v>19353</v>
       </c>
       <c r="F29" t="n">
-        <v>2489</v>
+        <v>471</v>
       </c>
       <c r="G29" t="n">
-        <v>17990</v>
+        <v>547</v>
       </c>
       <c r="H29" t="n">
-        <v>4168</v>
-      </c>
-      <c r="I29" t="inlineStr"/>
+        <v>387</v>
+      </c>
+      <c r="I29" t="n">
+        <v>8441</v>
+      </c>
       <c r="J29" t="n">
-        <v>15717</v>
+        <v>5124</v>
       </c>
       <c r="K29" t="n">
-        <v>2727</v>
+        <v>491</v>
       </c>
       <c r="L29" t="n">
-        <v>4386</v>
+        <v>3892</v>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>legislative</t>
+        </is>
       </c>
     </row>
     <row r="30">
@@ -1526,31 +1673,34 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E30" t="n">
-        <v>78942</v>
-      </c>
-      <c r="F30" t="n">
-        <v>1764</v>
-      </c>
+        <v>12325</v>
+      </c>
+      <c r="F30" t="inlineStr"/>
       <c r="G30" t="n">
-        <v>28313</v>
+        <v>2302</v>
       </c>
       <c r="H30" t="n">
-        <v>3157</v>
+        <v>318</v>
       </c>
       <c r="I30" t="n">
-        <v>5885</v>
+        <v>808</v>
       </c>
       <c r="J30" t="n">
-        <v>26794</v>
+        <v>4119</v>
       </c>
       <c r="K30" t="n">
-        <v>2364</v>
+        <v>293</v>
       </c>
       <c r="L30" t="n">
-        <v>10665</v>
+        <v>4485</v>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
       </c>
     </row>
     <row r="31">
@@ -1566,29 +1716,34 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E31" t="n">
-        <v>80191</v>
+        <v>12622</v>
       </c>
       <c r="F31" t="n">
-        <v>2150</v>
+        <v>178</v>
       </c>
       <c r="G31" t="n">
-        <v>23336</v>
+        <v>1944</v>
       </c>
       <c r="H31" t="n">
-        <v>3582</v>
+        <v>442</v>
       </c>
       <c r="I31" t="inlineStr"/>
       <c r="J31" t="n">
-        <v>38943</v>
+        <v>5884</v>
       </c>
       <c r="K31" t="n">
-        <v>5060</v>
+        <v>602</v>
       </c>
       <c r="L31" t="n">
-        <v>7120</v>
+        <v>3572</v>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
       </c>
     </row>
     <row r="32">
@@ -1596,7 +1751,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="2" t="n">
-        <v>39591</v>
+        <v>42848</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1604,29 +1759,34 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E32" t="n">
-        <v>45968</v>
-      </c>
-      <c r="F32" t="inlineStr"/>
+        <v>20698</v>
+      </c>
+      <c r="F32" t="n">
+        <v>1392</v>
+      </c>
       <c r="G32" t="n">
-        <v>7851</v>
-      </c>
-      <c r="H32" t="n">
-        <v>1114</v>
-      </c>
+        <v>849</v>
+      </c>
+      <c r="H32" t="inlineStr"/>
       <c r="I32" t="n">
-        <v>3972</v>
+        <v>6568</v>
       </c>
       <c r="J32" t="n">
-        <v>23768</v>
+        <v>10448</v>
       </c>
       <c r="K32" t="n">
-        <v>1678</v>
+        <v>916</v>
       </c>
       <c r="L32" t="n">
-        <v>7585</v>
+        <v>525</v>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>president</t>
+        </is>
       </c>
     </row>
     <row r="33">
@@ -1634,7 +1794,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="2" t="n">
-        <v>41723</v>
+        <v>42897</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1642,29 +1802,36 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E33" t="n">
-        <v>47741</v>
+        <v>13666</v>
       </c>
       <c r="F33" t="n">
-        <v>497</v>
+        <v>389</v>
       </c>
       <c r="G33" t="n">
-        <v>6197</v>
+        <v>452</v>
       </c>
       <c r="H33" t="n">
-        <v>1103</v>
-      </c>
-      <c r="I33" t="inlineStr"/>
+        <v>355</v>
+      </c>
+      <c r="I33" t="n">
+        <v>6959</v>
+      </c>
       <c r="J33" t="n">
-        <v>30100</v>
+        <v>3219</v>
       </c>
       <c r="K33" t="n">
-        <v>2865</v>
+        <v>344</v>
       </c>
       <c r="L33" t="n">
-        <v>6979</v>
+        <v>1948</v>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>legislative</t>
+        </is>
       </c>
     </row>
     <row r="34">
@@ -1680,31 +1847,36 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E34" t="n">
-        <v>49965</v>
+        <v>20643</v>
       </c>
       <c r="F34" t="n">
-        <v>568</v>
+        <v>602</v>
       </c>
       <c r="G34" t="n">
-        <v>18089</v>
+        <v>10163</v>
       </c>
       <c r="H34" t="n">
-        <v>2279</v>
+        <v>1299</v>
       </c>
       <c r="I34" t="n">
-        <v>4935</v>
+        <v>1659</v>
       </c>
       <c r="J34" t="n">
-        <v>22002</v>
+        <v>6353</v>
       </c>
       <c r="K34" t="n">
-        <v>2092</v>
+        <v>567</v>
       </c>
       <c r="L34" t="n">
         <v>0</v>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
       </c>
     </row>
     <row r="35">
@@ -1720,29 +1892,34 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E35" t="n">
-        <v>50128</v>
+        <v>20751</v>
       </c>
       <c r="F35" t="n">
-        <v>1544</v>
+        <v>772</v>
       </c>
       <c r="G35" t="n">
-        <v>12727</v>
+        <v>8125</v>
       </c>
       <c r="H35" t="n">
-        <v>3302</v>
+        <v>1663</v>
       </c>
       <c r="I35" t="inlineStr"/>
       <c r="J35" t="n">
-        <v>26836</v>
+        <v>8181</v>
       </c>
       <c r="K35" t="n">
-        <v>3234</v>
+        <v>1010</v>
       </c>
       <c r="L35" t="n">
-        <v>2485</v>
+        <v>1000</v>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
       </c>
     </row>
     <row r="36">
@@ -1750,7 +1927,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="2" t="n">
-        <v>39591</v>
+        <v>42848</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1758,31 +1935,34 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E36" t="n">
-        <v>52044</v>
+        <v>32940</v>
       </c>
       <c r="F36" t="n">
-        <v>3302</v>
+        <v>4783</v>
       </c>
       <c r="G36" t="n">
-        <v>25791</v>
-      </c>
-      <c r="H36" t="n">
-        <v>5392</v>
-      </c>
+        <v>3163</v>
+      </c>
+      <c r="H36" t="inlineStr"/>
       <c r="I36" t="n">
-        <v>3482</v>
+        <v>14029</v>
       </c>
       <c r="J36" t="n">
-        <v>10018</v>
+        <v>8879</v>
       </c>
       <c r="K36" t="n">
-        <v>1823</v>
+        <v>1092</v>
       </c>
       <c r="L36" t="n">
-        <v>2236</v>
+        <v>994</v>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>president</t>
+        </is>
       </c>
     </row>
     <row r="37">
@@ -1790,7 +1970,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="2" t="n">
-        <v>41723</v>
+        <v>42897</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1798,29 +1978,36 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E37" t="n">
-        <v>51029</v>
+        <v>23305</v>
       </c>
       <c r="F37" t="n">
-        <v>3668</v>
+        <v>1834</v>
       </c>
       <c r="G37" t="n">
-        <v>20338</v>
+        <v>3050</v>
       </c>
       <c r="H37" t="n">
-        <v>6457</v>
-      </c>
-      <c r="I37" t="inlineStr"/>
+        <v>1530</v>
+      </c>
+      <c r="I37" t="n">
+        <v>10116</v>
+      </c>
       <c r="J37" t="n">
-        <v>12879</v>
+        <v>4134</v>
       </c>
       <c r="K37" t="n">
-        <v>3460</v>
+        <v>494</v>
       </c>
       <c r="L37" t="n">
-        <v>4227</v>
+        <v>2147</v>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>legislative</t>
+        </is>
       </c>
     </row>
     <row r="38">
@@ -1836,31 +2023,36 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>47460</v>
+        <v>28359</v>
       </c>
       <c r="F38" t="n">
-        <v>2710</v>
+        <v>2158</v>
       </c>
       <c r="G38" t="n">
-        <v>24744</v>
+        <v>13766</v>
       </c>
       <c r="H38" t="n">
-        <v>3963</v>
+        <v>2564</v>
       </c>
       <c r="I38" t="n">
-        <v>3238</v>
+        <v>2348</v>
       </c>
       <c r="J38" t="n">
-        <v>10130</v>
+        <v>4513</v>
       </c>
       <c r="K38" t="n">
-        <v>1725</v>
+        <v>837</v>
       </c>
       <c r="L38" t="n">
-        <v>950</v>
+        <v>2173</v>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
       </c>
     </row>
     <row r="39">
@@ -1876,29 +2068,34 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>46307</v>
+        <v>26993</v>
       </c>
       <c r="F39" t="n">
-        <v>3295</v>
+        <v>1730</v>
       </c>
       <c r="G39" t="n">
-        <v>19533</v>
+        <v>11973</v>
       </c>
       <c r="H39" t="n">
-        <v>5956</v>
+        <v>3102</v>
       </c>
       <c r="I39" t="inlineStr"/>
       <c r="J39" t="n">
-        <v>11932</v>
+        <v>5798</v>
       </c>
       <c r="K39" t="n">
-        <v>3678</v>
+        <v>1460</v>
       </c>
       <c r="L39" t="n">
-        <v>1913</v>
+        <v>2930</v>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
       </c>
     </row>
     <row r="40">
@@ -1906,7 +2103,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="2" t="n">
-        <v>39591</v>
+        <v>42848</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1914,31 +2111,34 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E40" t="n">
-        <v>56285</v>
+        <v>44766</v>
       </c>
       <c r="F40" t="n">
-        <v>4776</v>
+        <v>11396</v>
       </c>
       <c r="G40" t="n">
-        <v>21568</v>
-      </c>
-      <c r="H40" t="n">
-        <v>5329</v>
-      </c>
+        <v>6343</v>
+      </c>
+      <c r="H40" t="inlineStr"/>
       <c r="I40" t="n">
-        <v>4114</v>
+        <v>16880</v>
       </c>
       <c r="J40" t="n">
-        <v>4076</v>
+        <v>6724</v>
       </c>
       <c r="K40" t="n">
-        <v>2033</v>
+        <v>1817</v>
       </c>
       <c r="L40" t="n">
-        <v>14389</v>
+        <v>1606</v>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>president</t>
+        </is>
       </c>
     </row>
     <row r="41">
@@ -1946,37 +2146,1802 @@
         <v>39</v>
       </c>
       <c r="B41" s="2" t="n">
+        <v>42897</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>10</v>
+      </c>
+      <c r="E41" t="n">
+        <v>31101</v>
+      </c>
+      <c r="F41" t="n">
+        <v>4202</v>
+      </c>
+      <c r="G41" t="n">
+        <v>3866</v>
+      </c>
+      <c r="H41" t="n">
+        <v>4551</v>
+      </c>
+      <c r="I41" t="n">
+        <v>12734</v>
+      </c>
+      <c r="J41" t="n">
+        <v>2280</v>
+      </c>
+      <c r="K41" t="n">
+        <v>900</v>
+      </c>
+      <c r="L41" t="n">
+        <v>2568</v>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>legislative</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" s="2" t="n">
+        <v>39591</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>11</v>
+      </c>
+      <c r="E42" t="n">
+        <v>47031</v>
+      </c>
+      <c r="F42" t="n">
+        <v>2672</v>
+      </c>
+      <c r="G42" t="n">
+        <v>25894</v>
+      </c>
+      <c r="H42" t="n">
+        <v>3726</v>
+      </c>
+      <c r="I42" t="n">
+        <v>4067</v>
+      </c>
+      <c r="J42" t="n">
+        <v>9315</v>
+      </c>
+      <c r="K42" t="n">
+        <v>1357</v>
+      </c>
+      <c r="L42" t="n">
+        <v>0</v>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" s="2" t="n">
         <v>41723</v>
       </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>Paris</t>
-        </is>
-      </c>
-      <c r="D41" t="n">
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>11</v>
+      </c>
+      <c r="E43" t="n">
+        <v>45861</v>
+      </c>
+      <c r="F43" t="n">
+        <v>2879</v>
+      </c>
+      <c r="G43" t="n">
+        <v>20524</v>
+      </c>
+      <c r="H43" t="n">
+        <v>5301</v>
+      </c>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="n">
+        <v>12304</v>
+      </c>
+      <c r="K43" t="n">
+        <v>2512</v>
+      </c>
+      <c r="L43" t="n">
+        <v>2341</v>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" s="2" t="n">
+        <v>42848</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>11</v>
+      </c>
+      <c r="E44" t="n">
+        <v>75237</v>
+      </c>
+      <c r="F44" t="n">
+        <v>17877</v>
+      </c>
+      <c r="G44" t="n">
+        <v>10247</v>
+      </c>
+      <c r="H44" t="inlineStr"/>
+      <c r="I44" t="n">
+        <v>29191</v>
+      </c>
+      <c r="J44" t="n">
+        <v>12136</v>
+      </c>
+      <c r="K44" t="n">
+        <v>3035</v>
+      </c>
+      <c r="L44" t="n">
+        <v>2751</v>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>president</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" s="2" t="n">
+        <v>42897</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>11</v>
+      </c>
+      <c r="E45" t="n">
+        <v>52299</v>
+      </c>
+      <c r="F45" t="n">
+        <v>7546</v>
+      </c>
+      <c r="G45" t="n">
+        <v>4521</v>
+      </c>
+      <c r="H45" t="n">
+        <v>6084</v>
+      </c>
+      <c r="I45" t="n">
+        <v>22419</v>
+      </c>
+      <c r="J45" t="n">
+        <v>3530</v>
+      </c>
+      <c r="K45" t="n">
+        <v>1335</v>
+      </c>
+      <c r="L45" t="n">
+        <v>6864</v>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>legislative</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" s="2" t="n">
+        <v>39591</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>12</v>
+      </c>
+      <c r="E46" t="n">
+        <v>53146</v>
+      </c>
+      <c r="F46" t="n">
+        <v>2324</v>
+      </c>
+      <c r="G46" t="n">
+        <v>24486</v>
+      </c>
+      <c r="H46" t="n">
+        <v>3125</v>
+      </c>
+      <c r="I46" t="n">
+        <v>5287</v>
+      </c>
+      <c r="J46" t="n">
+        <v>12922</v>
+      </c>
+      <c r="K46" t="n">
+        <v>1550</v>
+      </c>
+      <c r="L46" t="n">
+        <v>3452</v>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" s="2" t="n">
+        <v>41723</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>12</v>
+      </c>
+      <c r="E47" t="n">
+        <v>49695</v>
+      </c>
+      <c r="F47" t="n">
+        <v>2678</v>
+      </c>
+      <c r="G47" t="n">
+        <v>18585</v>
+      </c>
+      <c r="H47" t="n">
+        <v>5001</v>
+      </c>
+      <c r="I47" t="inlineStr"/>
+      <c r="J47" t="n">
+        <v>16569</v>
+      </c>
+      <c r="K47" t="n">
+        <v>3362</v>
+      </c>
+      <c r="L47" t="n">
+        <v>3500</v>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" s="2" t="n">
+        <v>42848</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>12</v>
+      </c>
+      <c r="E48" t="n">
+        <v>75050</v>
+      </c>
+      <c r="F48" t="n">
+        <v>15613</v>
+      </c>
+      <c r="G48" t="n">
+        <v>8614</v>
+      </c>
+      <c r="H48" t="inlineStr"/>
+      <c r="I48" t="n">
+        <v>26942</v>
+      </c>
+      <c r="J48" t="n">
+        <v>15918</v>
+      </c>
+      <c r="K48" t="n">
+        <v>4385</v>
+      </c>
+      <c r="L48" t="n">
+        <v>3578</v>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>president</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" s="2" t="n">
+        <v>42897</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>12</v>
+      </c>
+      <c r="E49" t="n">
+        <v>52590</v>
+      </c>
+      <c r="F49" t="n">
+        <v>6755</v>
+      </c>
+      <c r="G49" t="n">
+        <v>7945</v>
+      </c>
+      <c r="H49" t="n">
+        <v>3502</v>
+      </c>
+      <c r="I49" t="n">
+        <v>21162</v>
+      </c>
+      <c r="J49" t="n">
+        <v>7782</v>
+      </c>
+      <c r="K49" t="n">
+        <v>1767</v>
+      </c>
+      <c r="L49" t="n">
+        <v>3677</v>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>legislative</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" s="2" t="n">
+        <v>39591</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>13</v>
+      </c>
+      <c r="E50" t="n">
+        <v>58837</v>
+      </c>
+      <c r="F50" t="n">
+        <v>4608</v>
+      </c>
+      <c r="G50" t="n">
+        <v>29324</v>
+      </c>
+      <c r="H50" t="n">
+        <v>3808</v>
+      </c>
+      <c r="I50" t="n">
+        <v>5320</v>
+      </c>
+      <c r="J50" t="n">
+        <v>12559</v>
+      </c>
+      <c r="K50" t="n">
+        <v>1989</v>
+      </c>
+      <c r="L50" t="n">
+        <v>1229</v>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" s="2" t="n">
+        <v>41723</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>13</v>
+      </c>
+      <c r="E51" t="n">
+        <v>56670</v>
+      </c>
+      <c r="F51" t="n">
+        <v>3326</v>
+      </c>
+      <c r="G51" t="n">
+        <v>25193</v>
+      </c>
+      <c r="H51" t="n">
+        <v>5567</v>
+      </c>
+      <c r="I51" t="inlineStr"/>
+      <c r="J51" t="n">
+        <v>14157</v>
+      </c>
+      <c r="K51" t="n">
+        <v>4229</v>
+      </c>
+      <c r="L51" t="n">
+        <v>4198</v>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" s="2" t="n">
+        <v>42848</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>13</v>
+      </c>
+      <c r="E52" t="n">
+        <v>88639</v>
+      </c>
+      <c r="F52" t="n">
+        <v>21681</v>
+      </c>
+      <c r="G52" t="n">
+        <v>10511</v>
+      </c>
+      <c r="H52" t="inlineStr"/>
+      <c r="I52" t="n">
+        <v>30719</v>
+      </c>
+      <c r="J52" t="n">
+        <v>15329</v>
+      </c>
+      <c r="K52" t="n">
+        <v>5745</v>
+      </c>
+      <c r="L52" t="n">
+        <v>4654</v>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>president</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" s="2" t="n">
+        <v>42897</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>13</v>
+      </c>
+      <c r="E53" t="n">
+        <v>59432</v>
+      </c>
+      <c r="F53" t="n">
+        <v>9039</v>
+      </c>
+      <c r="G53" t="n">
+        <v>6487</v>
+      </c>
+      <c r="H53" t="n">
+        <v>5496</v>
+      </c>
+      <c r="I53" t="n">
+        <v>23025</v>
+      </c>
+      <c r="J53" t="n">
+        <v>5933</v>
+      </c>
+      <c r="K53" t="n">
+        <v>2609</v>
+      </c>
+      <c r="L53" t="n">
+        <v>6843</v>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>legislative</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" s="2" t="n">
+        <v>39591</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>14</v>
+      </c>
+      <c r="E54" t="n">
+        <v>48193</v>
+      </c>
+      <c r="F54" t="n">
+        <v>1806</v>
+      </c>
+      <c r="G54" t="n">
+        <v>21699</v>
+      </c>
+      <c r="H54" t="n">
+        <v>3871</v>
+      </c>
+      <c r="I54" t="n">
+        <v>6711</v>
+      </c>
+      <c r="J54" t="n">
+        <v>11465</v>
+      </c>
+      <c r="K54" t="n">
+        <v>1457</v>
+      </c>
+      <c r="L54" t="n">
+        <v>1184</v>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" s="2" t="n">
+        <v>41723</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>14</v>
+      </c>
+      <c r="E55" t="n">
+        <v>47477</v>
+      </c>
+      <c r="F55" t="n">
+        <v>2489</v>
+      </c>
+      <c r="G55" t="n">
+        <v>17990</v>
+      </c>
+      <c r="H55" t="n">
+        <v>4168</v>
+      </c>
+      <c r="I55" t="inlineStr"/>
+      <c r="J55" t="n">
+        <v>15717</v>
+      </c>
+      <c r="K55" t="n">
+        <v>2727</v>
+      </c>
+      <c r="L55" t="n">
+        <v>4386</v>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" s="2" t="n">
+        <v>42848</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>14</v>
+      </c>
+      <c r="E56" t="n">
+        <v>69461</v>
+      </c>
+      <c r="F56" t="n">
+        <v>13382</v>
+      </c>
+      <c r="G56" t="n">
+        <v>8003</v>
+      </c>
+      <c r="H56" t="inlineStr"/>
+      <c r="I56" t="n">
+        <v>25834</v>
+      </c>
+      <c r="J56" t="n">
+        <v>15475</v>
+      </c>
+      <c r="K56" t="n">
+        <v>3711</v>
+      </c>
+      <c r="L56" t="n">
+        <v>3056</v>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>president</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" s="2" t="n">
+        <v>42897</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>14</v>
+      </c>
+      <c r="E57" t="n">
+        <v>49176</v>
+      </c>
+      <c r="F57" t="n">
+        <v>5045</v>
+      </c>
+      <c r="G57" t="n">
+        <v>7195</v>
+      </c>
+      <c r="H57" t="n">
+        <v>3734</v>
+      </c>
+      <c r="I57" t="n">
+        <v>19877</v>
+      </c>
+      <c r="J57" t="n">
+        <v>7193</v>
+      </c>
+      <c r="K57" t="n">
+        <v>1614</v>
+      </c>
+      <c r="L57" t="n">
+        <v>4518</v>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>legislative</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" s="2" t="n">
+        <v>39591</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>15</v>
+      </c>
+      <c r="E58" t="n">
+        <v>78942</v>
+      </c>
+      <c r="F58" t="n">
+        <v>1764</v>
+      </c>
+      <c r="G58" t="n">
+        <v>28313</v>
+      </c>
+      <c r="H58" t="n">
+        <v>3157</v>
+      </c>
+      <c r="I58" t="n">
+        <v>5885</v>
+      </c>
+      <c r="J58" t="n">
+        <v>26794</v>
+      </c>
+      <c r="K58" t="n">
+        <v>2364</v>
+      </c>
+      <c r="L58" t="n">
+        <v>10665</v>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" s="2" t="n">
+        <v>41723</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>15</v>
+      </c>
+      <c r="E59" t="n">
+        <v>80191</v>
+      </c>
+      <c r="F59" t="n">
+        <v>2150</v>
+      </c>
+      <c r="G59" t="n">
+        <v>23336</v>
+      </c>
+      <c r="H59" t="n">
+        <v>3582</v>
+      </c>
+      <c r="I59" t="inlineStr"/>
+      <c r="J59" t="n">
+        <v>38943</v>
+      </c>
+      <c r="K59" t="n">
+        <v>5060</v>
+      </c>
+      <c r="L59" t="n">
+        <v>7120</v>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" s="2" t="n">
+        <v>42848</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>15</v>
+      </c>
+      <c r="E60" t="n">
+        <v>118947</v>
+      </c>
+      <c r="F60" t="n">
+        <v>15608</v>
+      </c>
+      <c r="G60" t="n">
+        <v>9085</v>
+      </c>
+      <c r="H60" t="inlineStr"/>
+      <c r="I60" t="n">
+        <v>42790</v>
+      </c>
+      <c r="J60" t="n">
+        <v>40235</v>
+      </c>
+      <c r="K60" t="n">
+        <v>6257</v>
+      </c>
+      <c r="L60" t="n">
+        <v>4972</v>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>president</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" s="2" t="n">
+        <v>42897</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>15</v>
+      </c>
+      <c r="E61" t="n">
+        <v>85143</v>
+      </c>
+      <c r="F61" t="n">
+        <v>5707</v>
+      </c>
+      <c r="G61" t="n">
+        <v>5669</v>
+      </c>
+      <c r="H61" t="n">
+        <v>3226</v>
+      </c>
+      <c r="I61" t="n">
+        <v>38346</v>
+      </c>
+      <c r="J61" t="n">
+        <v>24396</v>
+      </c>
+      <c r="K61" t="n">
+        <v>2678</v>
+      </c>
+      <c r="L61" t="n">
+        <v>5121</v>
+      </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>legislative</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" s="2" t="n">
+        <v>39591</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>16</v>
+      </c>
+      <c r="E62" t="n">
+        <v>45968</v>
+      </c>
+      <c r="F62" t="inlineStr"/>
+      <c r="G62" t="n">
+        <v>7851</v>
+      </c>
+      <c r="H62" t="n">
+        <v>1114</v>
+      </c>
+      <c r="I62" t="n">
+        <v>3972</v>
+      </c>
+      <c r="J62" t="n">
+        <v>23768</v>
+      </c>
+      <c r="K62" t="n">
+        <v>1678</v>
+      </c>
+      <c r="L62" t="n">
+        <v>7585</v>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" s="2" t="n">
+        <v>41723</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>16</v>
+      </c>
+      <c r="E63" t="n">
+        <v>47741</v>
+      </c>
+      <c r="F63" t="n">
+        <v>497</v>
+      </c>
+      <c r="G63" t="n">
+        <v>6197</v>
+      </c>
+      <c r="H63" t="n">
+        <v>1103</v>
+      </c>
+      <c r="I63" t="inlineStr"/>
+      <c r="J63" t="n">
+        <v>30100</v>
+      </c>
+      <c r="K63" t="n">
+        <v>2865</v>
+      </c>
+      <c r="L63" t="n">
+        <v>6979</v>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" s="2" t="n">
+        <v>42848</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>16</v>
+      </c>
+      <c r="E64" t="n">
+        <v>79954</v>
+      </c>
+      <c r="F64" t="n">
+        <v>4315</v>
+      </c>
+      <c r="G64" t="n">
+        <v>2353</v>
+      </c>
+      <c r="H64" t="inlineStr"/>
+      <c r="I64" t="n">
+        <v>21304</v>
+      </c>
+      <c r="J64" t="n">
+        <v>46734</v>
+      </c>
+      <c r="K64" t="n">
+        <v>3273</v>
+      </c>
+      <c r="L64" t="n">
+        <v>1975</v>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>president</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" s="2" t="n">
+        <v>42897</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>16</v>
+      </c>
+      <c r="E65" t="n">
+        <v>51079</v>
+      </c>
+      <c r="F65" t="n">
+        <v>1161</v>
+      </c>
+      <c r="G65" t="n">
+        <v>1157</v>
+      </c>
+      <c r="H65" t="n">
+        <v>803</v>
+      </c>
+      <c r="I65" t="n">
+        <v>22759</v>
+      </c>
+      <c r="J65" t="n">
+        <v>19453</v>
+      </c>
+      <c r="K65" t="n">
+        <v>1675</v>
+      </c>
+      <c r="L65" t="n">
+        <v>4071</v>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>legislative</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" s="2" t="n">
+        <v>39591</v>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>17</v>
+      </c>
+      <c r="E66" t="n">
+        <v>49965</v>
+      </c>
+      <c r="F66" t="n">
+        <v>568</v>
+      </c>
+      <c r="G66" t="n">
+        <v>18089</v>
+      </c>
+      <c r="H66" t="n">
+        <v>2279</v>
+      </c>
+      <c r="I66" t="n">
+        <v>4935</v>
+      </c>
+      <c r="J66" t="n">
+        <v>22002</v>
+      </c>
+      <c r="K66" t="n">
+        <v>2092</v>
+      </c>
+      <c r="L66" t="n">
+        <v>0</v>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" s="2" t="n">
+        <v>41723</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>17</v>
+      </c>
+      <c r="E67" t="n">
+        <v>50128</v>
+      </c>
+      <c r="F67" t="n">
+        <v>1544</v>
+      </c>
+      <c r="G67" t="n">
+        <v>12727</v>
+      </c>
+      <c r="H67" t="n">
+        <v>3302</v>
+      </c>
+      <c r="I67" t="inlineStr"/>
+      <c r="J67" t="n">
+        <v>26836</v>
+      </c>
+      <c r="K67" t="n">
+        <v>3234</v>
+      </c>
+      <c r="L67" t="n">
+        <v>2485</v>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" s="2" t="n">
+        <v>42848</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>17</v>
+      </c>
+      <c r="E68" t="n">
+        <v>82482</v>
+      </c>
+      <c r="F68" t="n">
+        <v>10677</v>
+      </c>
+      <c r="G68" t="n">
+        <v>5669</v>
+      </c>
+      <c r="H68" t="inlineStr"/>
+      <c r="I68" t="n">
+        <v>28423</v>
+      </c>
+      <c r="J68" t="n">
+        <v>31103</v>
+      </c>
+      <c r="K68" t="n">
+        <v>3786</v>
+      </c>
+      <c r="L68" t="n">
+        <v>2824</v>
+      </c>
+      <c r="M68" t="inlineStr">
+        <is>
+          <t>president</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" s="2" t="n">
+        <v>42897</v>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>17</v>
+      </c>
+      <c r="E69" t="n">
+        <v>56199</v>
+      </c>
+      <c r="F69" t="n">
+        <v>4142</v>
+      </c>
+      <c r="G69" t="n">
+        <v>4227</v>
+      </c>
+      <c r="H69" t="n">
+        <v>2040</v>
+      </c>
+      <c r="I69" t="n">
+        <v>26291</v>
+      </c>
+      <c r="J69" t="n">
+        <v>14701</v>
+      </c>
+      <c r="K69" t="n">
+        <v>1655</v>
+      </c>
+      <c r="L69" t="n">
+        <v>3143</v>
+      </c>
+      <c r="M69" t="inlineStr">
+        <is>
+          <t>legislative</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" s="2" t="n">
+        <v>39591</v>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>18</v>
+      </c>
+      <c r="E70" t="n">
+        <v>52044</v>
+      </c>
+      <c r="F70" t="n">
+        <v>3302</v>
+      </c>
+      <c r="G70" t="n">
+        <v>25791</v>
+      </c>
+      <c r="H70" t="n">
+        <v>5392</v>
+      </c>
+      <c r="I70" t="n">
+        <v>3482</v>
+      </c>
+      <c r="J70" t="n">
+        <v>10018</v>
+      </c>
+      <c r="K70" t="n">
+        <v>1823</v>
+      </c>
+      <c r="L70" t="n">
+        <v>2236</v>
+      </c>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" s="2" t="n">
+        <v>41723</v>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>18</v>
+      </c>
+      <c r="E71" t="n">
+        <v>51029</v>
+      </c>
+      <c r="F71" t="n">
+        <v>3668</v>
+      </c>
+      <c r="G71" t="n">
+        <v>20338</v>
+      </c>
+      <c r="H71" t="n">
+        <v>6457</v>
+      </c>
+      <c r="I71" t="inlineStr"/>
+      <c r="J71" t="n">
+        <v>12879</v>
+      </c>
+      <c r="K71" t="n">
+        <v>3460</v>
+      </c>
+      <c r="L71" t="n">
+        <v>4227</v>
+      </c>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" s="2" t="n">
+        <v>42848</v>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>18</v>
+      </c>
+      <c r="E72" t="n">
+        <v>84099</v>
+      </c>
+      <c r="F72" t="n">
+        <v>23867</v>
+      </c>
+      <c r="G72" t="n">
+        <v>11211</v>
+      </c>
+      <c r="H72" t="inlineStr"/>
+      <c r="I72" t="n">
+        <v>28437</v>
+      </c>
+      <c r="J72" t="n">
+        <v>12222</v>
+      </c>
+      <c r="K72" t="n">
+        <v>4595</v>
+      </c>
+      <c r="L72" t="n">
+        <v>3767</v>
+      </c>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>president</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" s="2" t="n">
+        <v>42897</v>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>18</v>
+      </c>
+      <c r="E73" t="n">
+        <v>54371</v>
+      </c>
+      <c r="F73" t="n">
+        <v>9339</v>
+      </c>
+      <c r="G73" t="n">
+        <v>8969</v>
+      </c>
+      <c r="H73" t="n">
+        <v>6474</v>
+      </c>
+      <c r="I73" t="n">
+        <v>6828</v>
+      </c>
+      <c r="J73" t="n">
+        <v>12097</v>
+      </c>
+      <c r="K73" t="n">
+        <v>2039</v>
+      </c>
+      <c r="L73" t="n">
+        <v>8625</v>
+      </c>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>legislative</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" s="2" t="n">
+        <v>39591</v>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>19</v>
+      </c>
+      <c r="E74" t="n">
+        <v>47460</v>
+      </c>
+      <c r="F74" t="n">
+        <v>2710</v>
+      </c>
+      <c r="G74" t="n">
+        <v>24744</v>
+      </c>
+      <c r="H74" t="n">
+        <v>3963</v>
+      </c>
+      <c r="I74" t="n">
+        <v>3238</v>
+      </c>
+      <c r="J74" t="n">
+        <v>10130</v>
+      </c>
+      <c r="K74" t="n">
+        <v>1725</v>
+      </c>
+      <c r="L74" t="n">
+        <v>950</v>
+      </c>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" s="2" t="n">
+        <v>41723</v>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>19</v>
+      </c>
+      <c r="E75" t="n">
+        <v>46307</v>
+      </c>
+      <c r="F75" t="n">
+        <v>3295</v>
+      </c>
+      <c r="G75" t="n">
+        <v>19533</v>
+      </c>
+      <c r="H75" t="n">
+        <v>5956</v>
+      </c>
+      <c r="I75" t="inlineStr"/>
+      <c r="J75" t="n">
+        <v>11932</v>
+      </c>
+      <c r="K75" t="n">
+        <v>3678</v>
+      </c>
+      <c r="L75" t="n">
+        <v>1913</v>
+      </c>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" s="2" t="n">
+        <v>42848</v>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>19</v>
+      </c>
+      <c r="E76" t="n">
+        <v>79665</v>
+      </c>
+      <c r="F76" t="n">
+        <v>24455</v>
+      </c>
+      <c r="G76" t="n">
+        <v>10352</v>
+      </c>
+      <c r="H76" t="inlineStr"/>
+      <c r="I76" t="n">
+        <v>23578</v>
+      </c>
+      <c r="J76" t="n">
+        <v>12977</v>
+      </c>
+      <c r="K76" t="n">
+        <v>4602</v>
+      </c>
+      <c r="L76" t="n">
+        <v>3701</v>
+      </c>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>president</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" s="2" t="n">
+        <v>42897</v>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>19</v>
+      </c>
+      <c r="E77" t="n">
+        <v>50024</v>
+      </c>
+      <c r="F77" t="n">
+        <v>9798</v>
+      </c>
+      <c r="G77" t="n">
+        <v>4488</v>
+      </c>
+      <c r="H77" t="n">
+        <v>5463</v>
+      </c>
+      <c r="I77" t="n">
+        <v>18429</v>
+      </c>
+      <c r="J77" t="n">
+        <v>3790</v>
+      </c>
+      <c r="K77" t="n">
+        <v>2129</v>
+      </c>
+      <c r="L77" t="n">
+        <v>5927</v>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>legislative</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" s="2" t="n">
+        <v>39591</v>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
         <v>20</v>
       </c>
-      <c r="E41" t="n">
+      <c r="E78" t="n">
+        <v>56285</v>
+      </c>
+      <c r="F78" t="n">
+        <v>4776</v>
+      </c>
+      <c r="G78" t="n">
+        <v>21568</v>
+      </c>
+      <c r="H78" t="n">
+        <v>5329</v>
+      </c>
+      <c r="I78" t="n">
+        <v>4114</v>
+      </c>
+      <c r="J78" t="n">
+        <v>4076</v>
+      </c>
+      <c r="K78" t="n">
+        <v>2033</v>
+      </c>
+      <c r="L78" t="n">
+        <v>14389</v>
+      </c>
+      <c r="M78" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" s="2" t="n">
+        <v>41723</v>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>20</v>
+      </c>
+      <c r="E79" t="n">
         <v>54966</v>
       </c>
-      <c r="F41" t="n">
+      <c r="F79" t="n">
         <v>5692</v>
       </c>
-      <c r="G41" t="n">
+      <c r="G79" t="n">
         <v>20502</v>
       </c>
-      <c r="H41" t="n">
+      <c r="H79" t="n">
         <v>5990</v>
       </c>
-      <c r="I41" t="inlineStr"/>
-      <c r="J41" t="n">
+      <c r="I79" t="inlineStr"/>
+      <c r="J79" t="n">
         <v>11467</v>
       </c>
-      <c r="K41" t="n">
+      <c r="K79" t="n">
         <v>4112</v>
       </c>
-      <c r="L41" t="n">
+      <c r="L79" t="n">
         <v>7203</v>
+      </c>
+      <c r="M79" t="inlineStr">
+        <is>
+          <t>municipale</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" s="2" t="n">
+        <v>42848</v>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>20</v>
+      </c>
+      <c r="E80" t="n">
+        <v>89574</v>
+      </c>
+      <c r="F80" t="n">
+        <v>28512</v>
+      </c>
+      <c r="G80" t="n">
+        <v>12469</v>
+      </c>
+      <c r="H80" t="inlineStr"/>
+      <c r="I80" t="n">
+        <v>27399</v>
+      </c>
+      <c r="J80" t="n">
+        <v>11451</v>
+      </c>
+      <c r="K80" t="n">
+        <v>5305</v>
+      </c>
+      <c r="L80" t="n">
+        <v>4438</v>
+      </c>
+      <c r="M80" t="inlineStr">
+        <is>
+          <t>president</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" s="2" t="n">
+        <v>42897</v>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>20</v>
+      </c>
+      <c r="E81" t="n">
+        <v>57413</v>
+      </c>
+      <c r="F81" t="n">
+        <v>11546</v>
+      </c>
+      <c r="G81" t="n">
+        <v>10700</v>
+      </c>
+      <c r="H81" t="n">
+        <v>7766</v>
+      </c>
+      <c r="I81" t="n">
+        <v>6505</v>
+      </c>
+      <c r="J81" t="n">
+        <v>4300</v>
+      </c>
+      <c r="K81" t="n">
+        <v>2446</v>
+      </c>
+      <c r="L81" t="n">
+        <v>14150</v>
+      </c>
+      <c r="M81" t="inlineStr">
+        <is>
+          <t>legislative</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>